<commit_message>
Success to read in letters and output win or loose game
</commit_message>
<xml_diff>
--- a/backlog3.xlsx
+++ b/backlog3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>As a/an</t>
   </si>
@@ -1024,7 +1024,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1081,8 +1081,8 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="5">
-        <v>0.4</v>
+      <c r="H2" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1108,7 +1108,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1283,7 +1283,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1392,7 +1392,7 @@
         <v>5</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.35">

</xml_diff>